<commit_message>
Updating with check for valid Email Address
</commit_message>
<xml_diff>
--- a/Customer Details.xlsx
+++ b/Customer Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mayank Tiwari\Documents\UiPath\UiPath RPA - Level 2 - Udemy\ExcelCustomersToWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCDB96DF-753C-483E-B490-C8C6BEAD575A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCEB1B1-80AA-4E67-BD9E-2667628AACD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A6D0A444-7708-4C2C-97B2-19C0A22FA6ED}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>First Name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>LastName5</t>
-  </si>
-  <si>
-    <t>$</t>
   </si>
   <si>
     <t>email5@serviceProvider5.com</t>
@@ -462,7 +459,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E1" sqref="E1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,11 +546,11 @@
       <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="1">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>